<commit_message>
update RTM  modify the Designs to be compatible with the updates
</commit_message>
<xml_diff>
--- a/Requirement/REQ_RTM.xlsx
+++ b/Requirement/REQ_RTM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maya Kind\Desktop\QA\Internet-Banking-System\Requirement\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263141B3-9521-4823-A064-138016A39014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -20,15 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>SRS-ID</t>
-  </si>
-  <si>
-    <t>Testcases</t>
-  </si>
-  <si>
-    <t>.tc1</t>
   </si>
   <si>
     <t>CST-REQ-ID</t>
@@ -226,12 +226,59 @@
   </si>
   <si>
     <t>Update RTM to be compatible with SRS &amp;SIQ changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DES_HL_ERD
+DES_HL_UseCas
+DES_HL_Decomposition
+</t>
+  </si>
+  <si>
+    <t>High Level Design</t>
+  </si>
+  <si>
+    <t>Low Level Design</t>
+  </si>
+  <si>
+    <t>DES_LL_WireframeUI_UserProfilePage</t>
+  </si>
+  <si>
+    <t>DES_LL_WireframeUI_LoginPage
+DES_LL_FlowChart_UserLogin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DES_LL_WireframeUI_RegisterPage
+DES_LL_FlowChart_UserRegistration
+</t>
+  </si>
+  <si>
+    <t>DES_LL_WireframeUI_AdminProfile
+DES_LL_FlowChart_AdminViewBalance
+DES_LL_FlowChart_AdminLogin
+DES_LL_FlowChart_DeleteUser
+DES_LL_FlowChart_AddBankAccount
+DES_LL_FlowChart_DeleteUser</t>
+  </si>
+  <si>
+    <t>v4.0</t>
+  </si>
+  <si>
+    <t>mayar</t>
+  </si>
+  <si>
+    <t>Update RTM  to add the Designs</t>
+  </si>
+  <si>
+    <t>v5.0</t>
+  </si>
+  <si>
+    <t>update RTM  modify the Designs to be compatible with the updates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -341,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,15 +434,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -423,8 +470,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -732,348 +786,645 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="43.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.36328125" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="E1" s="23"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F1" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="22"/>
+    </row>
+    <row r="3" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22"/>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22"/>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22"/>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22"/>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22"/>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25"/>
       <c r="B8" s="3"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="22"/>
+    </row>
+    <row r="10" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+    </row>
+    <row r="11" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="3"/>
       <c r="C11" s="12"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+    </row>
+    <row r="12" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="22"/>
+    </row>
+    <row r="13" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+    </row>
+    <row r="14" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="27"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+    </row>
+    <row r="15" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+    </row>
+    <row r="16" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="22"/>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="27"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+    </row>
+    <row r="17" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="19"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="22"/>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="27"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+    </row>
+    <row r="19" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="22"/>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+    </row>
+    <row r="20" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="27"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+    </row>
+    <row r="21" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+    </row>
+    <row r="22" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C22" s="30"/>
-    </row>
-    <row r="23" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+    </row>
+    <row r="23" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="3"/>
       <c r="C23" s="9"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+    </row>
+    <row r="24" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="22"/>
+    </row>
+    <row r="25" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+    </row>
+    <row r="26" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+    </row>
+    <row r="27" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="22"/>
       <c r="B27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="21"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+    </row>
+    <row r="28" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="22"/>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+    </row>
+    <row r="29" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+    </row>
+    <row r="30" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="22"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="21"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B30" s="21"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+    </row>
+    <row r="31" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="22"/>
       <c r="B31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="21"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+    </row>
+    <row r="32" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="C32" s="17"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+    </row>
+    <row r="33" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="C33" s="17"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+    </row>
+    <row r="34" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="3"/>
       <c r="C34" s="9"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+    </row>
+    <row r="35" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="10"/>
       <c r="C35" s="4"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="31"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+    </row>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+    </row>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+    </row>
+    <row r="51" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+    </row>
+    <row r="52" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+    </row>
+    <row r="53" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+    </row>
+    <row r="54" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+    </row>
+    <row r="55" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+    </row>
+    <row r="56" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+    </row>
+    <row r="57" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F57" s="31"/>
+      <c r="G57" s="31"/>
+    </row>
+    <row r="58" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F58" s="31"/>
+      <c r="G58" s="31"/>
+    </row>
+    <row r="59" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
+    </row>
+    <row r="60" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F60" s="31"/>
+      <c r="G60" s="31"/>
+    </row>
+    <row r="61" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F61" s="31"/>
+      <c r="G61" s="31"/>
+    </row>
+    <row r="62" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F62" s="31"/>
+      <c r="G62" s="31"/>
+    </row>
+    <row r="63" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F63" s="31"/>
+      <c r="G63" s="31"/>
+    </row>
+    <row r="64" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F64" s="31"/>
+      <c r="G64" s="31"/>
+    </row>
+    <row r="65" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F65" s="31"/>
+      <c r="G65" s="31"/>
+    </row>
+    <row r="66" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F66" s="31"/>
+      <c r="G66" s="31"/>
+    </row>
+    <row r="67" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F67" s="31"/>
+      <c r="G67" s="31"/>
+    </row>
+    <row r="68" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F68" s="31"/>
+      <c r="G68" s="31"/>
+    </row>
+    <row r="69" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F69" s="31"/>
+      <c r="G69" s="31"/>
+    </row>
+    <row r="70" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F70" s="31"/>
+      <c r="G70" s="31"/>
+    </row>
+    <row r="71" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F71" s="31"/>
+      <c r="G71" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="24">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G8"/>
+    <mergeCell ref="F9:G11"/>
+    <mergeCell ref="F12:G23"/>
+    <mergeCell ref="F24:G34"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E34"/>
+    <mergeCell ref="D36:E36"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="C29:C31"/>
     <mergeCell ref="A29:A31"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="A24:A28"/>
@@ -1083,7 +1434,6 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1091,75 +1441,103 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
-    <col min="4" max="4" width="46.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="46.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="16" customFormat="1" ht="15.65" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="16" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="16" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>40</v>
       </c>
       <c r="B2" s="15">
         <v>45508</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>65</v>
       </c>
-      <c r="C4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="15">
+        <v>45386</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="15">
+        <v>45423</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>